<commit_message>
Actualizar dashboard Odoo vs Mora y datos
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/odoo/odoo_pagos_mensuales.xlsx
+++ b/odoo/odoo_pagos_mensuales.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,801 +462,393 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>30.76</v>
+        <v>3114.1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>38.5</v>
+        <v>2802.81</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>104</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>38.5</v>
+        <v>4943.08</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>191</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>38.5</v>
+        <v>6425.47</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>38.5</v>
+        <v>2003.97</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>38.5</v>
+        <v>1009</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>38.5</v>
+        <v>871.71</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>38.5</v>
+        <v>2613.63</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>38.5</v>
+        <v>1332.19</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>72.40000000000001</v>
+        <v>3161.49</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>158.61</v>
+        <v>3628.15</v>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>166.35</v>
+        <v>2091.19</v>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>166.35</v>
+        <v>2282.29</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
-        <v>166.35</v>
+        <v>2268.02</v>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>166.35</v>
+        <v>580.65</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B17" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>127.85</v>
+        <v>7013.2</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>243</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B18" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>183.3</v>
+        <v>7772.85</v>
       </c>
       <c r="D18" t="n">
-        <v>7</v>
+        <v>264</v>
       </c>
       <c r="E18" t="n">
-        <v>7</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B19" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>277.25</v>
+        <v>5361.69</v>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>188</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" t="n">
-        <v>277.25</v>
+        <v>2665.15</v>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B21" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C21" t="n">
-        <v>200.25</v>
+        <v>3329.75</v>
       </c>
       <c r="D21" t="n">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="B22" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C22" t="n">
-        <v>277.25</v>
+        <v>1009</v>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C23" t="n">
-        <v>599.0700000000001</v>
+        <v>340.45</v>
       </c>
       <c r="D23" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E23" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C24" t="n">
-        <v>794.72</v>
+        <v>2534.64</v>
       </c>
       <c r="D24" t="n">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="E24" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B25" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1062.77</v>
-      </c>
-      <c r="D25" t="n">
-        <v>42</v>
-      </c>
-      <c r="E25" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B26" t="n">
-        <v>4</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1389.2</v>
-      </c>
-      <c r="D26" t="n">
-        <v>55</v>
-      </c>
-      <c r="E26" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B27" t="n">
-        <v>5</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1974.25</v>
-      </c>
-      <c r="D27" t="n">
-        <v>74</v>
-      </c>
-      <c r="E27" t="n">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B28" t="n">
-        <v>6</v>
-      </c>
-      <c r="C28" t="n">
-        <v>2582.53</v>
-      </c>
-      <c r="D28" t="n">
-        <v>96</v>
-      </c>
-      <c r="E28" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B29" t="n">
-        <v>7</v>
-      </c>
-      <c r="C29" t="n">
-        <v>3814.58</v>
-      </c>
-      <c r="D29" t="n">
-        <v>143</v>
-      </c>
-      <c r="E29" t="n">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B30" t="n">
-        <v>8</v>
-      </c>
-      <c r="C30" t="n">
-        <v>5142.34</v>
-      </c>
-      <c r="D30" t="n">
-        <v>195</v>
-      </c>
-      <c r="E30" t="n">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B31" t="n">
-        <v>9</v>
-      </c>
-      <c r="C31" t="n">
-        <v>10141.09</v>
-      </c>
-      <c r="D31" t="n">
-        <v>368</v>
-      </c>
-      <c r="E31" t="n">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B32" t="n">
-        <v>10</v>
-      </c>
-      <c r="C32" t="n">
-        <v>31590.01</v>
-      </c>
-      <c r="D32" t="n">
-        <v>1111</v>
-      </c>
-      <c r="E32" t="n">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B33" t="n">
-        <v>11</v>
-      </c>
-      <c r="C33" t="n">
-        <v>30958.17</v>
-      </c>
-      <c r="D33" t="n">
-        <v>1092</v>
-      </c>
-      <c r="E33" t="n">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B34" t="n">
-        <v>12</v>
-      </c>
-      <c r="C34" t="n">
-        <v>30594.74</v>
-      </c>
-      <c r="D34" t="n">
-        <v>1079</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>26850.95</v>
-      </c>
-      <c r="D35" t="n">
-        <v>941</v>
-      </c>
-      <c r="E35" t="n">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B36" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" t="n">
-        <v>14283.16</v>
-      </c>
-      <c r="D36" t="n">
-        <v>488</v>
-      </c>
-      <c r="E36" t="n">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1415.35</v>
-      </c>
-      <c r="D37" t="n">
-        <v>54</v>
-      </c>
-      <c r="E37" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B38" t="n">
-        <v>4</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1010.25</v>
-      </c>
-      <c r="D38" t="n">
         <v>39</v>
-      </c>
-      <c r="E38" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B39" t="n">
-        <v>5</v>
-      </c>
-      <c r="C39" t="n">
-        <v>843.9</v>
-      </c>
-      <c r="D39" t="n">
-        <v>33</v>
-      </c>
-      <c r="E39" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B40" t="n">
-        <v>6</v>
-      </c>
-      <c r="C40" t="n">
-        <v>774.64</v>
-      </c>
-      <c r="D40" t="n">
-        <v>31</v>
-      </c>
-      <c r="E40" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B41" t="n">
-        <v>7</v>
-      </c>
-      <c r="C41" t="n">
-        <v>437.33</v>
-      </c>
-      <c r="D41" t="n">
-        <v>17</v>
-      </c>
-      <c r="E41" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B42" t="n">
-        <v>8</v>
-      </c>
-      <c r="C42" t="n">
-        <v>475.83</v>
-      </c>
-      <c r="D42" t="n">
-        <v>18</v>
-      </c>
-      <c r="E42" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B43" t="n">
-        <v>9</v>
-      </c>
-      <c r="C43" t="n">
-        <v>475.83</v>
-      </c>
-      <c r="D43" t="n">
-        <v>18</v>
-      </c>
-      <c r="E43" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B44" t="n">
-        <v>10</v>
-      </c>
-      <c r="C44" t="n">
-        <v>475.83</v>
-      </c>
-      <c r="D44" t="n">
-        <v>18</v>
-      </c>
-      <c r="E44" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B45" t="n">
-        <v>11</v>
-      </c>
-      <c r="C45" t="n">
-        <v>475.83</v>
-      </c>
-      <c r="D45" t="n">
-        <v>18</v>
-      </c>
-      <c r="E45" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B46" t="n">
-        <v>12</v>
-      </c>
-      <c r="C46" t="n">
-        <v>441.93</v>
-      </c>
-      <c r="D46" t="n">
-        <v>16</v>
-      </c>
-      <c r="E46" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>2027</v>
-      </c>
-      <c r="B47" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" t="n">
-        <v>55.45</v>
-      </c>
-      <c r="D47" t="n">
-        <v>2</v>
-      </c>
-      <c r="E47" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>2027</v>
-      </c>
-      <c r="B48" t="n">
-        <v>2</v>
-      </c>
-      <c r="C48" t="n">
-        <v>16.95</v>
-      </c>
-      <c r="D48" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar scripts Odoo vs Mora, dashboard y datos
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/odoo/odoo_pagos_mensuales.xlsx
+++ b/odoo/odoo_pagos_mensuales.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
         <v>2025</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>3114.1</v>
+        <v>25033.76</v>
       </c>
       <c r="D2" t="n">
-        <v>117</v>
+        <v>868</v>
       </c>
       <c r="E2" t="n">
-        <v>92</v>
+        <v>835</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>2025</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>2802.81</v>
+        <v>26653.55</v>
       </c>
       <c r="D3" t="n">
-        <v>104</v>
+        <v>922</v>
       </c>
       <c r="E3" t="n">
-        <v>92</v>
+        <v>876</v>
       </c>
     </row>
     <row r="4">
@@ -499,356 +499,50 @@
         <v>2025</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>4943.08</v>
+        <v>19853.08</v>
       </c>
       <c r="D4" t="n">
-        <v>191</v>
+        <v>694</v>
       </c>
       <c r="E4" t="n">
-        <v>107</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>6425.47</v>
+        <v>34878.35</v>
       </c>
       <c r="D5" t="n">
-        <v>215</v>
+        <v>1224</v>
       </c>
       <c r="E5" t="n">
-        <v>182</v>
+        <v>956</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>2003.97</v>
+        <v>16890.23</v>
       </c>
       <c r="D6" t="n">
-        <v>67</v>
+        <v>576</v>
       </c>
       <c r="E6" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1009</v>
-      </c>
-      <c r="D7" t="n">
-        <v>43</v>
-      </c>
-      <c r="E7" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="n">
-        <v>871.71</v>
-      </c>
-      <c r="D8" t="n">
-        <v>29</v>
-      </c>
-      <c r="E8" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2613.63</v>
-      </c>
-      <c r="D9" t="n">
-        <v>88</v>
-      </c>
-      <c r="E9" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1332.19</v>
-      </c>
-      <c r="D10" t="n">
-        <v>47</v>
-      </c>
-      <c r="E10" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3161.49</v>
-      </c>
-      <c r="D11" t="n">
-        <v>109</v>
-      </c>
-      <c r="E11" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3628.15</v>
-      </c>
-      <c r="D12" t="n">
-        <v>113</v>
-      </c>
-      <c r="E12" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>2025</v>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2091.19</v>
-      </c>
-      <c r="D13" t="n">
-        <v>69</v>
-      </c>
-      <c r="E13" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2282.29</v>
-      </c>
-      <c r="D14" t="n">
-        <v>80</v>
-      </c>
-      <c r="E14" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B15" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" t="n">
-        <v>2268.02</v>
-      </c>
-      <c r="D15" t="n">
-        <v>78</v>
-      </c>
-      <c r="E15" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B16" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" t="n">
-        <v>580.65</v>
-      </c>
-      <c r="D16" t="n">
-        <v>19</v>
-      </c>
-      <c r="E16" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B17" t="n">
-        <v>5</v>
-      </c>
-      <c r="C17" t="n">
-        <v>7013.2</v>
-      </c>
-      <c r="D17" t="n">
-        <v>243</v>
-      </c>
-      <c r="E17" t="n">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B18" t="n">
-        <v>6</v>
-      </c>
-      <c r="C18" t="n">
-        <v>7772.85</v>
-      </c>
-      <c r="D18" t="n">
-        <v>264</v>
-      </c>
-      <c r="E18" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B19" t="n">
-        <v>7</v>
-      </c>
-      <c r="C19" t="n">
-        <v>5361.69</v>
-      </c>
-      <c r="D19" t="n">
-        <v>188</v>
-      </c>
-      <c r="E19" t="n">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B20" t="n">
-        <v>8</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2665.15</v>
-      </c>
-      <c r="D20" t="n">
-        <v>85</v>
-      </c>
-      <c r="E20" t="n">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B21" t="n">
-        <v>9</v>
-      </c>
-      <c r="C21" t="n">
-        <v>3329.75</v>
-      </c>
-      <c r="D21" t="n">
-        <v>107</v>
-      </c>
-      <c r="E21" t="n">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B22" t="n">
-        <v>10</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1009</v>
-      </c>
-      <c r="D22" t="n">
-        <v>43</v>
-      </c>
-      <c r="E22" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B23" t="n">
-        <v>11</v>
-      </c>
-      <c r="C23" t="n">
-        <v>340.45</v>
-      </c>
-      <c r="D23" t="n">
-        <v>15</v>
-      </c>
-      <c r="E23" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B24" t="n">
-        <v>12</v>
-      </c>
-      <c r="C24" t="n">
-        <v>2534.64</v>
-      </c>
-      <c r="D24" t="n">
-        <v>87</v>
-      </c>
-      <c r="E24" t="n">
-        <v>39</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>